<commit_message>
Extraction des tableaux du word
</commit_message>
<xml_diff>
--- a/mon_ficheir.xlsx
+++ b/mon_ficheir.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,12 +436,7 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Population de l’année 2019</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Population de l’année 2019_1</t>
+          <t>Rapport de masculinité</t>
         </is>
       </c>
     </row>
@@ -451,12 +446,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>7066</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>5761</t>
+          <t>122,7</t>
         </is>
       </c>
     </row>

</xml_diff>